<commit_message>
cc planting dates viz
</commit_message>
<xml_diff>
--- a/data/raw/byhand_cover-crop-planting-dates.xlsx
+++ b/data/raw/byhand_cover-crop-planting-dates.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\au757887\PC_documents\_git-it\ghproj_CENTS\data\raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gina\Documents\_git-it\ghproj_CENTS\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2076CAAD-769E-4000-A080-2D696DDACE4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E89D8E-3DD7-42FB-AF2D-78D883D592DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{12D20B23-4266-411A-B6D5-0A20568D073A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{12D20B23-4266-411A-B6D5-0A20568D073A}"/>
   </bookViews>
   <sheets>
-    <sheet name="sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="ccplanting" sheetId="1" r:id="rId1"/>
+    <sheet name="ccterminating" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="30">
   <si>
     <t>day</t>
   </si>
@@ -53,12 +54,6 @@
     <t>mix_M</t>
   </si>
   <si>
-    <t>radish_M</t>
-  </si>
-  <si>
-    <t>radish_L</t>
-  </si>
-  <si>
     <t>cctrt_id</t>
   </si>
   <si>
@@ -71,20 +66,84 @@
     <t>08</t>
   </si>
   <si>
-    <t>05</t>
-  </si>
-  <si>
     <t>09</t>
+  </si>
+  <si>
+    <t>activity</t>
+  </si>
+  <si>
+    <t>planting</t>
+  </si>
+  <si>
+    <t>till_id</t>
+  </si>
+  <si>
+    <t>termination</t>
+  </si>
+  <si>
+    <t>notill</t>
+  </si>
+  <si>
+    <t>med</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>These are exact dates of planting taken from Eugene's info</t>
+  </si>
+  <si>
+    <t>These are not exact and need to be updated once I talk with Eugene</t>
+  </si>
+  <si>
+    <t>The high tillage plots were tilled in the fall, terminating the ccs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The med and no-till plots weren't touched the fall before, were sprayed and tilled the </t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>2019</t>
+  </si>
+  <si>
+    <t>2020</t>
+  </si>
+  <si>
+    <t>rad_L</t>
+  </si>
+  <si>
+    <t>rad_M</t>
+  </si>
+  <si>
+    <t>est_year</t>
+  </si>
+  <si>
+    <t>2018</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -110,7 +169,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -118,6 +177,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,147 +512,396 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8094B07-BF52-4219-AD74-BA183E27208A}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="14.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22" style="2" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="22" style="2" customWidth="1"/>
-    <col min="4" max="4" width="28.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="14.77734375" style="1"/>
+    <col min="1" max="1" width="14.81640625" style="1"/>
+    <col min="2" max="2" width="22" style="2" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" style="2" customWidth="1"/>
+    <col min="4" max="5" width="22" style="2" customWidth="1"/>
+    <col min="6" max="6" width="28.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="14.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="2">
+        <v>23</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="2">
+        <v>2018</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="2">
+        <v>16</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
+      <c r="D8" s="2">
+        <v>2018</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="2">
+        <v>16</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="2">
+        <v>2018</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="2">
+        <v>20</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="2">
+        <v>2018</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="2">
+        <v>2019</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2">
+        <v>31</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="2">
+        <v>2019</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2">
+        <v>31</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="2">
+        <v>2019</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="2">
+        <v>2019</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A87D539-7A70-4483-9BC5-DEA88670C2EF}">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>2018</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <v>2018</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9">
+        <v>2018</v>
+      </c>
+      <c r="D9" s="2">
+        <v>2018</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="2">
-        <v>2018</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10">
+        <v>2019</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11">
+        <v>2019</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="2">
-        <v>2018</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
-        <v>16</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="2">
-        <v>2018</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
-        <v>20</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="2">
-        <v>2018</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="2">
+      <c r="C12">
         <v>2019</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
-        <v>31</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="2">
+      <c r="D12" s="2">
         <v>2019</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
-        <v>31</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="2">
-        <v>2019</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="2">
-        <v>2019</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="E12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
milestone before erasing things
</commit_message>
<xml_diff>
--- a/data/raw/byhand_cover-crop-planting-dates.xlsx
+++ b/data/raw/byhand_cover-crop-planting-dates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gina\Documents\_git-it\ghproj_CENTS\data\raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\au757887\PC_documents\_git-it\ghproj_CENTS\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E89D8E-3DD7-42FB-AF2D-78D883D592DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4CDAE29-B786-4ABA-B927-8601EC766D88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{12D20B23-4266-411A-B6D5-0A20568D073A}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{12D20B23-4266-411A-B6D5-0A20568D073A}"/>
   </bookViews>
   <sheets>
     <sheet name="ccplanting" sheetId="1" r:id="rId1"/>
@@ -84,12 +84,6 @@
     <t>notill</t>
   </si>
   <si>
-    <t>med</t>
-  </si>
-  <si>
-    <t>high</t>
-  </si>
-  <si>
     <t>These are exact dates of planting taken from Eugene's info</t>
   </si>
   <si>
@@ -127,6 +121,12 @@
   </si>
   <si>
     <t>2018</t>
+  </si>
+  <si>
+    <t>noninversion</t>
+  </si>
+  <si>
+    <t>inversion</t>
   </si>
 </sst>
 </file>
@@ -514,27 +514,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8094B07-BF52-4219-AD74-BA183E27208A}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="14.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.81640625" style="1"/>
+    <col min="1" max="1" width="14.77734375" style="1"/>
     <col min="2" max="2" width="22" style="2" customWidth="1"/>
-    <col min="3" max="3" width="18.453125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="18.44140625" style="2" customWidth="1"/>
     <col min="4" max="5" width="22" style="2" customWidth="1"/>
-    <col min="6" max="6" width="28.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="14.81640625" style="1"/>
+    <col min="6" max="6" width="28.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="14.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -548,13 +548,13 @@
         <v>2</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -568,13 +568,13 @@
         <v>2018</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -588,13 +588,13 @@
         <v>2018</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -608,13 +608,13 @@
         <v>2018</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -628,13 +628,13 @@
         <v>2018</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -648,13 +648,13 @@
         <v>2019</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -668,13 +668,13 @@
         <v>2019</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -688,13 +688,13 @@
         <v>2019</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -708,10 +708,10 @@
         <v>2019</v>
       </c>
       <c r="E14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -723,31 +723,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A87D539-7A70-4483-9BC5-DEA88670C2EF}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.36328125" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -755,7 +755,7 @@
         <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>2</v>
@@ -767,7 +767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -778,41 +778,41 @@
         <v>2018</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="C8">
         <v>2018</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="C9">
         <v>2018</v>
@@ -821,13 +821,13 @@
         <v>2018</v>
       </c>
       <c r="E9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -838,41 +838,41 @@
         <v>2019</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="C11">
         <v>2019</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="C12">
         <v>2019</v>
@@ -881,13 +881,13 @@
         <v>2019</v>
       </c>
       <c r="E12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -895,7 +895,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>

</xml_diff>